<commit_message>
added first MVP version
</commit_message>
<xml_diff>
--- a/recipe_db.xlsx
+++ b/recipe_db.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="374" documentId="11_15D4434B7C403DBADFA4E62351F0958B69545958" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9749B6EE-E081-48EB-B187-ED5D14ECB00E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="99">
   <si>
     <t>code</t>
   </si>
@@ -87,9 +88,6 @@
     <t>kolendra</t>
   </si>
   <si>
-    <t>pieruszka</t>
-  </si>
-  <si>
     <t>soda oczyszczona</t>
   </si>
   <si>
@@ -214,12 +212,114 @@
   </si>
   <si>
     <t>salad</t>
+  </si>
+  <si>
+    <t>intermeal</t>
+  </si>
+  <si>
+    <t>Kotlet schabowy w ziołach</t>
+  </si>
+  <si>
+    <t>schab</t>
+  </si>
+  <si>
+    <t>Surówka z marchewkii pestek dyni</t>
+  </si>
+  <si>
+    <t>pestki dyni</t>
+  </si>
+  <si>
+    <t>cytryna</t>
+  </si>
+  <si>
+    <t>Zupa jarzynowa z fasolą szparagową</t>
+  </si>
+  <si>
+    <t>pietruszka</t>
+  </si>
+  <si>
+    <t>fasolka szparagowa</t>
+  </si>
+  <si>
+    <t>Krupnik wegetariański</t>
+  </si>
+  <si>
+    <t>seler</t>
+  </si>
+  <si>
+    <t>kasza gryczana</t>
+  </si>
+  <si>
+    <t>grzyby suszone</t>
+  </si>
+  <si>
+    <t>liść laurowy</t>
+  </si>
+  <si>
+    <t>ziele angielskie</t>
+  </si>
+  <si>
+    <t>Rukola z indykiemi prażonymi pestkami dyni</t>
+  </si>
+  <si>
+    <t>pierś z indyka</t>
+  </si>
+  <si>
+    <t>peski dyni</t>
+  </si>
+  <si>
+    <t>szczypiorek</t>
+  </si>
+  <si>
+    <t>Mozarella z pomidorami</t>
+  </si>
+  <si>
+    <t>pomidor</t>
+  </si>
+  <si>
+    <t>bazylia</t>
+  </si>
+  <si>
+    <t>szpinak</t>
+  </si>
+  <si>
+    <t>oliwka</t>
+  </si>
+  <si>
+    <t>Zupa koperkowa</t>
+  </si>
+  <si>
+    <t>ziemniak</t>
+  </si>
+  <si>
+    <t>koperek</t>
+  </si>
+  <si>
+    <t>Barszcz czerwony</t>
+  </si>
+  <si>
+    <t>burak</t>
+  </si>
+  <si>
+    <t>majeranek</t>
+  </si>
+  <si>
+    <t>Zupa krem z cukini</t>
+  </si>
+  <si>
+    <t>porcja rosołowa</t>
+  </si>
+  <si>
+    <t>cukinia</t>
+  </si>
+  <si>
+    <t>mozarella</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -260,6 +360,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -308,7 +411,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,9 +444,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,6 +496,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -551,22 +688,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N86" sqref="N86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,22 +720,25 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
       </c>
       <c r="J1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -629,8 +769,17 @@
       <c r="J2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -655,8 +804,17 @@
       <c r="J3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -681,8 +839,17 @@
       <c r="J4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -707,8 +874,17 @@
       <c r="J5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
@@ -733,8 +909,17 @@
       <c r="J6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -759,8 +944,17 @@
       <c r="J7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -785,8 +979,11 @@
       <c r="J8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -817,8 +1014,17 @@
       <c r="J9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
@@ -843,8 +1049,17 @@
       <c r="J10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
@@ -869,8 +1084,17 @@
       <c r="J11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
@@ -895,16 +1119,25 @@
       <c r="J12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -921,8 +1154,17 @@
       <c r="J13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -947,8 +1189,17 @@
       <c r="J14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
@@ -973,10 +1224,19 @@
       <c r="J15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -999,10 +1259,19 @@
       <c r="J16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -1025,14 +1294,23 @@
       <c r="J17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
       <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
       <c r="E18">
         <v>1</v>
       </c>
@@ -1051,16 +1329,19 @@
       <c r="J18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -1083,8 +1364,17 @@
       <c r="J19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
@@ -1109,10 +1399,19 @@
       <c r="J20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -1135,8 +1434,17 @@
       <c r="J21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
@@ -1161,13 +1469,22 @@
       <c r="J22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23">
         <v>0.5</v>
@@ -1187,36 +1504,54 @@
       <c r="J23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
       <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
         <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>34</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -1239,13 +1574,22 @@
       <c r="J25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
       <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
         <v>35</v>
-      </c>
-      <c r="D26" t="s">
-        <v>36</v>
       </c>
       <c r="E26">
         <v>0.5</v>
@@ -1265,16 +1609,19 @@
       <c r="J26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>4</v>
       </c>
       <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
         <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
       </c>
       <c r="D27" t="s">
         <v>19</v>
@@ -1297,10 +1644,19 @@
       <c r="J27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
         <v>19</v>
@@ -1323,10 +1679,19 @@
       <c r="J28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
         <v>21</v>
@@ -1349,13 +1714,22 @@
       <c r="J29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1375,8 +1749,17 @@
       <c r="J30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
       <c r="C31" t="s">
         <v>20</v>
       </c>
@@ -1401,10 +1784,19 @@
       <c r="J31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
@@ -1427,10 +1819,19 @@
       <c r="J32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -1453,39 +1854,57 @@
       <c r="J33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
       <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
         <v>44</v>
       </c>
-      <c r="D34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G34" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>45</v>
-      </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -1505,36 +1924,54 @@
       <c r="J35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
       <c r="C36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
         <v>46</v>
-      </c>
-      <c r="D36" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>47</v>
       </c>
       <c r="D37" t="s">
         <v>16</v>
@@ -1557,10 +1994,19 @@
       <c r="J37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
@@ -1583,10 +2029,19 @@
       <c r="J38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D39" t="s">
         <v>16</v>
@@ -1609,8 +2064,17 @@
       <c r="J39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
       <c r="C40" t="s">
         <v>22</v>
       </c>
@@ -1635,10 +2099,19 @@
       <c r="J40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
         <v>16</v>
@@ -1661,16 +2134,19 @@
       <c r="J41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" t="s">
         <v>21</v>
@@ -1693,10 +2169,19 @@
       <c r="J42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43" t="s">
         <v>21</v>
@@ -1719,10 +2204,19 @@
       <c r="J43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>54</v>
+      </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1745,14 +2239,23 @@
       <c r="J44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>54</v>
+      </c>
       <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
         <v>56</v>
       </c>
-      <c r="D45" t="s">
-        <v>57</v>
-      </c>
       <c r="E45">
         <v>1</v>
       </c>
@@ -1771,13 +2274,22 @@
       <c r="J45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1797,19 +2309,22 @@
       <c r="J46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
         <v>58</v>
       </c>
-      <c r="C47" t="s">
-        <v>59</v>
-      </c>
       <c r="D47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1821,18 +2336,27 @@
         <v>0</v>
       </c>
       <c r="H47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
       </c>
       <c r="J47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
         <v>21</v>
@@ -1847,44 +2371,62 @@
         <v>0</v>
       </c>
       <c r="H48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
       </c>
       <c r="J48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
       <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49">
+        <v>0.5</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
         <v>60</v>
-      </c>
-      <c r="D49" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="b">
-        <v>0</v>
-      </c>
-      <c r="G49" t="b">
-        <v>0</v>
-      </c>
-      <c r="H49" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>61</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
@@ -1899,13 +2441,2396 @@
         <v>0</v>
       </c>
       <c r="H50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
       </c>
       <c r="J50" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>125</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58">
+        <v>0.5</v>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59">
+        <v>0.25</v>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62">
+        <v>4</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" t="b">
+        <v>1</v>
+      </c>
+      <c r="K62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" t="b">
+        <v>1</v>
+      </c>
+      <c r="K63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64">
+        <v>200</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" t="b">
+        <v>1</v>
+      </c>
+      <c r="K64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65">
+        <v>0.5</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+      <c r="J65" t="b">
+        <v>1</v>
+      </c>
+      <c r="K65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" t="b">
+        <v>1</v>
+      </c>
+      <c r="K66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" t="b">
+        <v>1</v>
+      </c>
+      <c r="K67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+      <c r="K68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" t="s">
+        <v>75</v>
+      </c>
+      <c r="D69" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69">
+        <v>0.5</v>
+      </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+      <c r="J69" t="b">
+        <v>1</v>
+      </c>
+      <c r="K69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+      <c r="J70" t="b">
+        <v>1</v>
+      </c>
+      <c r="K70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71">
+        <v>0.5</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" t="b">
+        <v>1</v>
+      </c>
+      <c r="K71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72">
+        <v>100</v>
+      </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72" t="b">
+        <v>1</v>
+      </c>
+      <c r="K72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" t="s">
+        <v>77</v>
+      </c>
+      <c r="D73" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73" t="b">
+        <v>1</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
+      <c r="J73" t="b">
+        <v>1</v>
+      </c>
+      <c r="K73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>10</v>
+      </c>
+      <c r="B74" t="s">
+        <v>74</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" t="b">
+        <v>0</v>
+      </c>
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+      <c r="K74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" t="s">
+        <v>78</v>
+      </c>
+      <c r="D75" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75" t="b">
+        <v>1</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+      <c r="J75" t="b">
+        <v>1</v>
+      </c>
+      <c r="K75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>10</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" t="s">
+        <v>79</v>
+      </c>
+      <c r="D76" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76">
+        <v>3</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" t="b">
+        <v>0</v>
+      </c>
+      <c r="J76" t="b">
+        <v>1</v>
+      </c>
+      <c r="K76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>10</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77">
+        <v>3</v>
+      </c>
+      <c r="F77" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J77" t="b">
+        <v>1</v>
+      </c>
+      <c r="K77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>10</v>
+      </c>
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" t="b">
+        <v>1</v>
+      </c>
+      <c r="K78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>11</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" t="s">
+        <v>55</v>
+      </c>
+      <c r="D79" t="s">
+        <v>56</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>1</v>
+      </c>
+      <c r="H79" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>11</v>
+      </c>
+      <c r="B80" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80" t="s">
+        <v>81</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80">
+        <v>125</v>
+      </c>
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+      <c r="H80" t="b">
+        <v>0</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>11</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" t="s">
+        <v>39</v>
+      </c>
+      <c r="D81" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81">
+        <v>0.5</v>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" t="b">
+        <v>1</v>
+      </c>
+      <c r="H81" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+      <c r="J81" t="b">
+        <v>0</v>
+      </c>
+      <c r="K81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>11</v>
+      </c>
+      <c r="B82" t="s">
+        <v>80</v>
+      </c>
+      <c r="C82" t="s">
+        <v>82</v>
+      </c>
+      <c r="D82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" t="b">
+        <v>1</v>
+      </c>
+      <c r="H82" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" t="b">
+        <v>0</v>
+      </c>
+      <c r="K82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>11</v>
+      </c>
+      <c r="B83" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83">
+        <v>0.5</v>
+      </c>
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" t="b">
+        <v>0</v>
+      </c>
+      <c r="K83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>12</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" t="s">
+        <v>98</v>
+      </c>
+      <c r="D84" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84">
+        <v>0.5</v>
+      </c>
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+      <c r="H84" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" t="b">
+        <v>0</v>
+      </c>
+      <c r="K84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>12</v>
+      </c>
+      <c r="B85" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" t="s">
+        <v>85</v>
+      </c>
+      <c r="D85" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" t="b">
+        <v>0</v>
+      </c>
+      <c r="I85" t="b">
+        <v>1</v>
+      </c>
+      <c r="J85" t="b">
+        <v>0</v>
+      </c>
+      <c r="K85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>12</v>
+      </c>
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+      <c r="C86" t="s">
+        <v>86</v>
+      </c>
+      <c r="D86" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86">
+        <v>0.25</v>
+      </c>
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" t="b">
+        <v>0</v>
+      </c>
+      <c r="K86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87" t="s">
+        <v>69</v>
+      </c>
+      <c r="D87" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="b">
+        <v>1</v>
+      </c>
+      <c r="H87" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" t="b">
+        <v>1</v>
+      </c>
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+      <c r="K87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>12</v>
+      </c>
+      <c r="B88" t="s">
+        <v>84</v>
+      </c>
+      <c r="C88" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" t="s">
+        <v>56</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" t="b">
+        <v>1</v>
+      </c>
+      <c r="H88" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" t="b">
+        <v>1</v>
+      </c>
+      <c r="J88" t="b">
+        <v>0</v>
+      </c>
+      <c r="K88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>12</v>
+      </c>
+      <c r="B89" t="s">
+        <v>84</v>
+      </c>
+      <c r="C89" t="s">
+        <v>60</v>
+      </c>
+      <c r="D89" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" t="b">
+        <v>0</v>
+      </c>
+      <c r="I89" t="b">
+        <v>1</v>
+      </c>
+      <c r="J89" t="b">
+        <v>0</v>
+      </c>
+      <c r="K89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>12</v>
+      </c>
+      <c r="B90" t="s">
+        <v>84</v>
+      </c>
+      <c r="C90" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90">
+        <v>4</v>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" t="b">
+        <v>0</v>
+      </c>
+      <c r="K90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>13</v>
+      </c>
+      <c r="B91" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91" t="s">
+        <v>81</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91">
+        <v>250</v>
+      </c>
+      <c r="F91" t="b">
+        <v>1</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+      <c r="H91" t="b">
+        <v>0</v>
+      </c>
+      <c r="I91" t="b">
+        <v>0</v>
+      </c>
+      <c r="J91" t="b">
+        <v>1</v>
+      </c>
+      <c r="K91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>13</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" t="s">
+        <v>90</v>
+      </c>
+      <c r="D92" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" t="b">
+        <v>0</v>
+      </c>
+      <c r="J92" t="b">
+        <v>1</v>
+      </c>
+      <c r="K92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>13</v>
+      </c>
+      <c r="B93" t="s">
+        <v>89</v>
+      </c>
+      <c r="C93" t="s">
+        <v>91</v>
+      </c>
+      <c r="D93" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93" t="b">
+        <v>1</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" t="b">
+        <v>0</v>
+      </c>
+      <c r="J93" t="b">
+        <v>1</v>
+      </c>
+      <c r="K93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>13</v>
+      </c>
+      <c r="B94" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94">
+        <v>4</v>
+      </c>
+      <c r="F94" t="b">
+        <v>1</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" t="b">
+        <v>0</v>
+      </c>
+      <c r="J94" t="b">
+        <v>1</v>
+      </c>
+      <c r="K94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>13</v>
+      </c>
+      <c r="B95" t="s">
+        <v>89</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" t="b">
+        <v>1</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" t="b">
+        <v>0</v>
+      </c>
+      <c r="J95" t="b">
+        <v>1</v>
+      </c>
+      <c r="K95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>13</v>
+      </c>
+      <c r="B96" t="s">
+        <v>89</v>
+      </c>
+      <c r="C96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" t="b">
+        <v>0</v>
+      </c>
+      <c r="J96" t="b">
+        <v>1</v>
+      </c>
+      <c r="K96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>13</v>
+      </c>
+      <c r="B97" t="s">
+        <v>89</v>
+      </c>
+      <c r="C97" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" t="s">
+        <v>21</v>
+      </c>
+      <c r="E97">
+        <v>3</v>
+      </c>
+      <c r="F97" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" t="b">
+        <v>0</v>
+      </c>
+      <c r="J97" t="b">
+        <v>1</v>
+      </c>
+      <c r="K97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>13</v>
+      </c>
+      <c r="B98" t="s">
+        <v>89</v>
+      </c>
+      <c r="C98" t="s">
+        <v>41</v>
+      </c>
+      <c r="D98" t="s">
+        <v>21</v>
+      </c>
+      <c r="E98">
+        <v>3</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" t="b">
+        <v>0</v>
+      </c>
+      <c r="J98" t="b">
+        <v>1</v>
+      </c>
+      <c r="K98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>13</v>
+      </c>
+      <c r="B99" t="s">
+        <v>89</v>
+      </c>
+      <c r="C99" t="s">
+        <v>72</v>
+      </c>
+      <c r="D99" t="s">
+        <v>21</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" t="b">
+        <v>0</v>
+      </c>
+      <c r="J99" t="b">
+        <v>1</v>
+      </c>
+      <c r="K99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>13</v>
+      </c>
+      <c r="B100" t="s">
+        <v>89</v>
+      </c>
+      <c r="C100" t="s">
+        <v>75</v>
+      </c>
+      <c r="D100" t="s">
+        <v>21</v>
+      </c>
+      <c r="E100">
+        <v>0.5</v>
+      </c>
+      <c r="F100" t="b">
+        <v>1</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" t="b">
+        <v>1</v>
+      </c>
+      <c r="K100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>14</v>
+      </c>
+      <c r="B101" t="s">
+        <v>92</v>
+      </c>
+      <c r="C101" t="s">
+        <v>93</v>
+      </c>
+      <c r="D101" t="s">
+        <v>21</v>
+      </c>
+      <c r="E101">
+        <v>3</v>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" t="b">
+        <v>1</v>
+      </c>
+      <c r="K101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>14</v>
+      </c>
+      <c r="B102" t="s">
+        <v>92</v>
+      </c>
+      <c r="C102" t="s">
+        <v>41</v>
+      </c>
+      <c r="D102" t="s">
+        <v>21</v>
+      </c>
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102" t="b">
+        <v>1</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+      <c r="I102" t="b">
+        <v>0</v>
+      </c>
+      <c r="J102" t="b">
+        <v>1</v>
+      </c>
+      <c r="K102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>14</v>
+      </c>
+      <c r="B103" t="s">
+        <v>92</v>
+      </c>
+      <c r="C103" t="s">
+        <v>72</v>
+      </c>
+      <c r="D103" t="s">
+        <v>21</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103" t="b">
+        <v>1</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+      <c r="I103" t="b">
+        <v>0</v>
+      </c>
+      <c r="J103" t="b">
+        <v>1</v>
+      </c>
+      <c r="K103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>14</v>
+      </c>
+      <c r="B104" t="s">
+        <v>92</v>
+      </c>
+      <c r="C104" t="s">
+        <v>75</v>
+      </c>
+      <c r="D104" t="s">
+        <v>21</v>
+      </c>
+      <c r="E104">
+        <v>0.25</v>
+      </c>
+      <c r="F104" t="b">
+        <v>1</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <v>0</v>
+      </c>
+      <c r="I104" t="b">
+        <v>0</v>
+      </c>
+      <c r="J104" t="b">
+        <v>1</v>
+      </c>
+      <c r="K104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
+        <v>92</v>
+      </c>
+      <c r="C105" t="s">
+        <v>78</v>
+      </c>
+      <c r="D105" t="s">
+        <v>21</v>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="F105" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" t="b">
+        <v>0</v>
+      </c>
+      <c r="J105" t="b">
+        <v>1</v>
+      </c>
+      <c r="K105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>14</v>
+      </c>
+      <c r="B106" t="s">
+        <v>92</v>
+      </c>
+      <c r="C106" t="s">
+        <v>79</v>
+      </c>
+      <c r="D106" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106">
+        <v>3</v>
+      </c>
+      <c r="F106" t="b">
+        <v>1</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" t="b">
+        <v>0</v>
+      </c>
+      <c r="J106" t="b">
+        <v>1</v>
+      </c>
+      <c r="K106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>92</v>
+      </c>
+      <c r="C107" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" t="s">
+        <v>21</v>
+      </c>
+      <c r="E107">
+        <v>3</v>
+      </c>
+      <c r="F107" t="b">
+        <v>1</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+      <c r="I107" t="b">
+        <v>0</v>
+      </c>
+      <c r="J107" t="b">
+        <v>1</v>
+      </c>
+      <c r="K107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>92</v>
+      </c>
+      <c r="C108" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108" t="s">
+        <v>13</v>
+      </c>
+      <c r="E108">
+        <v>2</v>
+      </c>
+      <c r="F108" t="b">
+        <v>1</v>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+      <c r="H108" t="b">
+        <v>0</v>
+      </c>
+      <c r="I108" t="b">
+        <v>0</v>
+      </c>
+      <c r="J108" t="b">
+        <v>1</v>
+      </c>
+      <c r="K108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>14</v>
+      </c>
+      <c r="B109" t="s">
+        <v>92</v>
+      </c>
+      <c r="C109" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109" t="b">
+        <v>0</v>
+      </c>
+      <c r="I109" t="b">
+        <v>0</v>
+      </c>
+      <c r="J109" t="b">
+        <v>1</v>
+      </c>
+      <c r="K109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
+        <v>92</v>
+      </c>
+      <c r="C110" t="s">
+        <v>70</v>
+      </c>
+      <c r="D110" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110">
+        <v>0.25</v>
+      </c>
+      <c r="F110" t="b">
+        <v>1</v>
+      </c>
+      <c r="G110" t="b">
+        <v>0</v>
+      </c>
+      <c r="H110" t="b">
+        <v>0</v>
+      </c>
+      <c r="I110" t="b">
+        <v>0</v>
+      </c>
+      <c r="J110" t="b">
+        <v>1</v>
+      </c>
+      <c r="K110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>14</v>
+      </c>
+      <c r="B111" t="s">
+        <v>92</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" t="s">
+        <v>11</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111" t="b">
+        <v>0</v>
+      </c>
+      <c r="I111" t="b">
+        <v>0</v>
+      </c>
+      <c r="J111" t="b">
+        <v>1</v>
+      </c>
+      <c r="K111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>15</v>
+      </c>
+      <c r="B112" t="s">
+        <v>95</v>
+      </c>
+      <c r="C112" t="s">
+        <v>96</v>
+      </c>
+      <c r="D112" t="s">
+        <v>21</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+      <c r="H112" t="b">
+        <v>0</v>
+      </c>
+      <c r="I112" t="b">
+        <v>0</v>
+      </c>
+      <c r="J112" t="b">
+        <v>1</v>
+      </c>
+      <c r="K112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>15</v>
+      </c>
+      <c r="B113" t="s">
+        <v>95</v>
+      </c>
+      <c r="C113" t="s">
+        <v>97</v>
+      </c>
+      <c r="D113" t="s">
+        <v>21</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" t="b">
+        <v>0</v>
+      </c>
+      <c r="I113" t="b">
+        <v>0</v>
+      </c>
+      <c r="J113" t="b">
+        <v>1</v>
+      </c>
+      <c r="K113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>15</v>
+      </c>
+      <c r="B114" t="s">
+        <v>95</v>
+      </c>
+      <c r="C114" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" t="s">
+        <v>13</v>
+      </c>
+      <c r="E114">
+        <v>2</v>
+      </c>
+      <c r="F114" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+      <c r="H114" t="b">
+        <v>0</v>
+      </c>
+      <c r="I114" t="b">
+        <v>0</v>
+      </c>
+      <c r="J114" t="b">
+        <v>1</v>
+      </c>
+      <c r="K114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>15</v>
+      </c>
+      <c r="B115" t="s">
+        <v>95</v>
+      </c>
+      <c r="C115" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115" t="b">
+        <v>1</v>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115" t="b">
+        <v>0</v>
+      </c>
+      <c r="I115" t="b">
+        <v>0</v>
+      </c>
+      <c r="J115" t="b">
+        <v>1</v>
+      </c>
+      <c r="K115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>15</v>
+      </c>
+      <c r="B116" t="s">
+        <v>95</v>
+      </c>
+      <c r="C116" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116" t="b">
+        <v>1</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
+      <c r="I116" t="b">
+        <v>0</v>
+      </c>
+      <c r="J116" t="b">
+        <v>1</v>
+      </c>
+      <c r="K116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>15</v>
+      </c>
+      <c r="B117" t="s">
+        <v>95</v>
+      </c>
+      <c r="C117" t="s">
+        <v>41</v>
+      </c>
+      <c r="D117" t="s">
+        <v>21</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117" t="b">
+        <v>1</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+      <c r="H117" t="b">
+        <v>0</v>
+      </c>
+      <c r="I117" t="b">
+        <v>0</v>
+      </c>
+      <c r="J117" t="b">
+        <v>1</v>
+      </c>
+      <c r="K117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>15</v>
+      </c>
+      <c r="B118" t="s">
+        <v>95</v>
+      </c>
+      <c r="C118" t="s">
+        <v>20</v>
+      </c>
+      <c r="D118" t="s">
+        <v>21</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118" t="b">
+        <v>1</v>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+      <c r="H118" t="b">
+        <v>0</v>
+      </c>
+      <c r="I118" t="b">
+        <v>0</v>
+      </c>
+      <c r="J118" t="b">
+        <v>1</v>
+      </c>
+      <c r="K118" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1914,24 +4839,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
buttons for data reload and excel export + textbox placeholder
</commit_message>
<xml_diff>
--- a/recipe_db.xlsx
+++ b/recipe_db.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBB30E3-EF98-49D0-A88A-6D27197666D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29020" windowHeight="15840"/>
+    <workbookView xWindow="30960" yWindow="2160" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$337</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="172">
   <si>
     <t>code</t>
   </si>
@@ -97,9 +101,6 @@
   </si>
   <si>
     <t>double_portion</t>
-  </si>
-  <si>
-    <t>pierś  z kurczaka</t>
   </si>
   <si>
     <t>por</t>
@@ -540,7 +541,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,7 +697,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -729,9 +730,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -764,6 +782,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -939,12 +974,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L337"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O279" sqref="O279"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,22 +1018,22 @@
         <v>26</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -1272,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
@@ -1310,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
@@ -1348,7 +1383,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -1386,7 +1421,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
@@ -1424,10 +1459,10 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>20</v>
@@ -1462,7 +1497,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
@@ -1500,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
@@ -1538,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
@@ -1576,7 +1611,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
@@ -1614,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
@@ -1652,10 +1687,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1690,7 +1725,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>19</v>
@@ -1728,10 +1763,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>20</v>
@@ -1766,7 +1801,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
@@ -1804,13 +1839,13 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="2">
         <v>0.5</v>
@@ -1842,10 +1877,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>25</v>
@@ -1880,10 +1915,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>11</v>
@@ -1918,13 +1953,13 @@
         <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E26" s="2">
         <v>0.5</v>
@@ -1956,10 +1991,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>18</v>
@@ -1994,10 +2029,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>18</v>
@@ -2032,10 +2067,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>20</v>
@@ -2070,13 +2105,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
@@ -2108,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>19</v>
@@ -2146,10 +2181,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>20</v>
@@ -2184,10 +2219,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>11</v>
@@ -2222,10 +2257,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>25</v>
@@ -2260,10 +2295,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>25</v>
@@ -2298,10 +2333,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>25</v>
@@ -2336,10 +2371,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>16</v>
@@ -2374,10 +2409,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>16</v>
@@ -2412,10 +2447,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>16</v>
@@ -2450,7 +2485,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>21</v>
@@ -2488,10 +2523,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>16</v>
@@ -2526,10 +2561,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>20</v>
@@ -2564,10 +2599,10 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>20</v>
@@ -2602,10 +2637,10 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -2640,13 +2675,13 @@
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E45" s="2">
         <v>1</v>
@@ -2678,10 +2713,10 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>25</v>
@@ -2716,13 +2751,13 @@
         <v>6</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E47" s="2">
         <v>1</v>
@@ -2754,10 +2789,10 @@
         <v>6</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>20</v>
@@ -2792,10 +2827,10 @@
         <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>20</v>
@@ -2830,10 +2865,10 @@
         <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>11</v>
@@ -2868,10 +2903,10 @@
         <v>7</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>6</v>
@@ -2906,10 +2941,10 @@
         <v>7</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>16</v>
@@ -2944,7 +2979,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>14</v>
@@ -2982,7 +3017,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>15</v>
@@ -3020,7 +3055,7 @@
         <v>7</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>23</v>
@@ -3058,10 +3093,10 @@
         <v>8</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>20</v>
@@ -3096,10 +3131,10 @@
         <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>11</v>
@@ -3134,10 +3169,10 @@
         <v>8</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>20</v>
@@ -3172,10 +3207,10 @@
         <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>11</v>
@@ -3210,7 +3245,7 @@
         <v>8</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>14</v>
@@ -3248,7 +3283,7 @@
         <v>8</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>15</v>
@@ -3286,10 +3321,10 @@
         <v>9</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>20</v>
@@ -3324,10 +3359,10 @@
         <v>9</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>20</v>
@@ -3362,10 +3397,10 @@
         <v>9</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
@@ -3400,10 +3435,10 @@
         <v>9</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>20</v>
@@ -3438,7 +3473,7 @@
         <v>9</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>14</v>
@@ -3476,7 +3511,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>15</v>
@@ -3514,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>20</v>
@@ -3552,10 +3587,10 @@
         <v>10</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>20</v>
@@ -3590,10 +3625,10 @@
         <v>10</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>20</v>
@@ -3628,10 +3663,10 @@
         <v>10</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>20</v>
@@ -3666,10 +3701,10 @@
         <v>10</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>6</v>
@@ -3704,10 +3739,10 @@
         <v>10</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>20</v>
@@ -3742,7 +3777,7 @@
         <v>10</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>12</v>
@@ -3780,10 +3815,10 @@
         <v>10</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>20</v>
@@ -3818,10 +3853,10 @@
         <v>10</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>20</v>
@@ -3856,7 +3891,7 @@
         <v>10</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>15</v>
@@ -3894,7 +3929,7 @@
         <v>10</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>14</v>
@@ -3932,13 +3967,13 @@
         <v>11</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E79" s="2">
         <v>2</v>
@@ -3970,10 +4005,10 @@
         <v>11</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>6</v>
@@ -4008,10 +4043,10 @@
         <v>11</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>20</v>
@@ -4046,10 +4081,10 @@
         <v>11</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>11</v>
@@ -4084,10 +4119,10 @@
         <v>11</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>11</v>
@@ -4122,10 +4157,10 @@
         <v>12</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>20</v>
@@ -4160,10 +4195,10 @@
         <v>12</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>20</v>
@@ -4198,10 +4233,10 @@
         <v>12</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>20</v>
@@ -4236,10 +4271,10 @@
         <v>12</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>11</v>
@@ -4274,13 +4309,13 @@
         <v>12</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E88" s="2">
         <v>1</v>
@@ -4312,10 +4347,10 @@
         <v>12</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>11</v>
@@ -4350,10 +4385,10 @@
         <v>12</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>20</v>
@@ -4388,10 +4423,10 @@
         <v>13</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>6</v>
@@ -4426,10 +4461,10 @@
         <v>13</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>20</v>
@@ -4464,10 +4499,10 @@
         <v>13</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>20</v>
@@ -4502,7 +4537,7 @@
         <v>13</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>10</v>
@@ -4540,10 +4575,10 @@
         <v>13</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>11</v>
@@ -4578,7 +4613,7 @@
         <v>13</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>14</v>
@@ -4616,7 +4651,7 @@
         <v>13</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>15</v>
@@ -4654,10 +4689,10 @@
         <v>13</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>20</v>
@@ -4692,10 +4727,10 @@
         <v>13</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>20</v>
@@ -4730,10 +4765,10 @@
         <v>13</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>20</v>
@@ -4768,10 +4803,10 @@
         <v>14</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>20</v>
@@ -4806,10 +4841,10 @@
         <v>14</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>20</v>
@@ -4844,10 +4879,10 @@
         <v>14</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>20</v>
@@ -4882,10 +4917,10 @@
         <v>14</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>20</v>
@@ -4920,10 +4955,10 @@
         <v>14</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>20</v>
@@ -4958,10 +4993,10 @@
         <v>14</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>20</v>
@@ -4996,7 +5031,7 @@
         <v>14</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>15</v>
@@ -5034,7 +5069,7 @@
         <v>14</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>12</v>
@@ -5072,10 +5107,10 @@
         <v>14</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>11</v>
@@ -5110,10 +5145,10 @@
         <v>14</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>20</v>
@@ -5148,7 +5183,7 @@
         <v>14</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>14</v>
@@ -5186,10 +5221,10 @@
         <v>15</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>20</v>
@@ -5224,10 +5259,10 @@
         <v>15</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>20</v>
@@ -5262,7 +5297,7 @@
         <v>15</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>12</v>
@@ -5300,7 +5335,7 @@
         <v>15</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>10</v>
@@ -5338,10 +5373,10 @@
         <v>15</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>11</v>
@@ -5376,10 +5411,10 @@
         <v>15</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>20</v>
@@ -5414,7 +5449,7 @@
         <v>15</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>19</v>
@@ -5452,10 +5487,10 @@
         <v>16</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>20</v>
@@ -5490,7 +5525,7 @@
         <v>16</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>23</v>
@@ -5528,10 +5563,10 @@
         <v>17</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>6</v>
@@ -5566,10 +5601,10 @@
         <v>18</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>6</v>
@@ -5604,7 +5639,7 @@
         <v>18</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>15</v>
@@ -5642,10 +5677,10 @@
         <v>18</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>20</v>
@@ -5680,10 +5715,10 @@
         <v>19</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>20</v>
@@ -5718,10 +5753,10 @@
         <v>19</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>20</v>
@@ -5756,10 +5791,10 @@
         <v>19</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>20</v>
@@ -5794,7 +5829,7 @@
         <v>19</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>10</v>
@@ -5832,7 +5867,7 @@
         <v>19</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>12</v>
@@ -5870,7 +5905,7 @@
         <v>19</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>14</v>
@@ -5908,7 +5943,7 @@
         <v>19</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>15</v>
@@ -5946,10 +5981,10 @@
         <v>20</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>20</v>
@@ -5984,10 +6019,10 @@
         <v>20</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>20</v>
@@ -6022,10 +6057,10 @@
         <v>20</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>20</v>
@@ -6060,10 +6095,10 @@
         <v>20</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>20</v>
@@ -6098,7 +6133,7 @@
         <v>20</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>14</v>
@@ -6136,7 +6171,7 @@
         <v>20</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>15</v>
@@ -6174,10 +6209,10 @@
         <v>20</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>20</v>
@@ -6212,10 +6247,10 @@
         <v>20</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>20</v>
@@ -6250,10 +6285,10 @@
         <v>21</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C140" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>6</v>
@@ -6288,13 +6323,13 @@
         <v>21</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E141" s="2">
         <v>2</v>
@@ -6326,10 +6361,10 @@
         <v>21</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>20</v>
@@ -6364,10 +6399,10 @@
         <v>21</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>20</v>
@@ -6402,10 +6437,10 @@
         <v>21</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>20</v>
@@ -6440,10 +6475,10 @@
         <v>21</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>20</v>
@@ -6478,10 +6513,10 @@
         <v>21</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>11</v>
@@ -6516,10 +6551,10 @@
         <v>21</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>25</v>
@@ -6554,10 +6589,10 @@
         <v>21</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>25</v>
@@ -6592,7 +6627,7 @@
         <v>21</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>14</v>
@@ -6630,7 +6665,7 @@
         <v>21</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>15</v>
@@ -6668,7 +6703,7 @@
         <v>22</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>8</v>
@@ -6706,10 +6741,10 @@
         <v>22</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>20</v>
@@ -6744,10 +6779,10 @@
         <v>22</v>
       </c>
       <c r="B153" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>20</v>
@@ -6782,10 +6817,10 @@
         <v>22</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>20</v>
@@ -6820,10 +6855,10 @@
         <v>22</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>20</v>
@@ -6858,10 +6893,10 @@
         <v>22</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>20</v>
@@ -6896,10 +6931,10 @@
         <v>23</v>
       </c>
       <c r="B157" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C157" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>20</v>
@@ -6934,10 +6969,10 @@
         <v>23</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>20</v>
@@ -6972,7 +7007,7 @@
         <v>23</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>19</v>
@@ -7010,7 +7045,7 @@
         <v>23</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>12</v>
@@ -7048,10 +7083,10 @@
         <v>23</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>20</v>
@@ -7086,10 +7121,10 @@
         <v>23</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>11</v>
@@ -7124,10 +7159,10 @@
         <v>23</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>25</v>
@@ -7162,13 +7197,13 @@
         <v>24</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E164" s="2">
         <v>1</v>
@@ -7200,10 +7235,10 @@
         <v>24</v>
       </c>
       <c r="B165" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C165" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>6</v>
@@ -7238,10 +7273,10 @@
         <v>24</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>20</v>
@@ -7276,10 +7311,10 @@
         <v>24</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>20</v>
@@ -7314,10 +7349,10 @@
         <v>24</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>11</v>
@@ -7352,10 +7387,10 @@
         <v>24</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>20</v>
@@ -7390,10 +7425,10 @@
         <v>24</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>20</v>
@@ -7428,7 +7463,7 @@
         <v>24</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>14</v>
@@ -7466,7 +7501,7 @@
         <v>24</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>15</v>
@@ -7504,10 +7539,10 @@
         <v>25</v>
       </c>
       <c r="B173" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C173" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>6</v>
@@ -7542,13 +7577,13 @@
         <v>25</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C174" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D174" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E174" s="2">
         <v>2</v>
@@ -7580,10 +7615,10 @@
         <v>25</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>20</v>
@@ -7618,10 +7653,10 @@
         <v>25</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>20</v>
@@ -7656,10 +7691,10 @@
         <v>25</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>11</v>
@@ -7694,10 +7729,10 @@
         <v>25</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>20</v>
@@ -7732,7 +7767,7 @@
         <v>25</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>14</v>
@@ -7770,7 +7805,7 @@
         <v>25</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>15</v>
@@ -7808,10 +7843,10 @@
         <v>26</v>
       </c>
       <c r="B181" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C181" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>20</v>
@@ -7846,10 +7881,10 @@
         <v>26</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>20</v>
@@ -7884,13 +7919,13 @@
         <v>26</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C183" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D183" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D183" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E183" s="2">
         <v>2</v>
@@ -7922,10 +7957,10 @@
         <v>26</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>11</v>
@@ -7960,10 +7995,10 @@
         <v>26</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>20</v>
@@ -7998,10 +8033,10 @@
         <v>26</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>20</v>
@@ -8036,10 +8071,10 @@
         <v>26</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>20</v>
@@ -8074,7 +8109,7 @@
         <v>26</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>15</v>
@@ -8112,7 +8147,7 @@
         <v>26</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>14</v>
@@ -8150,10 +8185,10 @@
         <v>26</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>20</v>
@@ -8188,10 +8223,10 @@
         <v>27</v>
       </c>
       <c r="B191" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C191" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>6</v>
@@ -8226,7 +8261,7 @@
         <v>27</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>19</v>
@@ -8264,10 +8299,10 @@
         <v>27</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>11</v>
@@ -8302,7 +8337,7 @@
         <v>27</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>14</v>
@@ -8340,7 +8375,7 @@
         <v>27</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>15</v>
@@ -8378,10 +8413,10 @@
         <v>28</v>
       </c>
       <c r="B196" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C196" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>6</v>
@@ -8416,10 +8451,10 @@
         <v>28</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>20</v>
@@ -8454,10 +8489,10 @@
         <v>28</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>20</v>
@@ -8492,10 +8527,10 @@
         <v>28</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>20</v>
@@ -8530,7 +8565,7 @@
         <v>28</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>19</v>
@@ -8568,10 +8603,10 @@
         <v>28</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>11</v>
@@ -8606,10 +8641,10 @@
         <v>28</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>20</v>
@@ -8644,7 +8679,7 @@
         <v>28</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>14</v>
@@ -8682,7 +8717,7 @@
         <v>28</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>15</v>
@@ -8720,10 +8755,10 @@
         <v>28</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>11</v>
@@ -8758,7 +8793,7 @@
         <v>29</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>9</v>
@@ -8796,10 +8831,10 @@
         <v>29</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>11</v>
@@ -8834,10 +8869,10 @@
         <v>29</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>18</v>
@@ -8872,7 +8907,7 @@
         <v>29</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>23</v>
@@ -8910,10 +8945,10 @@
         <v>29</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>16</v>
@@ -8948,7 +8983,7 @@
         <v>29</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>14</v>
@@ -8986,7 +9021,7 @@
         <v>29</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>15</v>
@@ -9024,13 +9059,13 @@
         <v>30</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C213" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="D213" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D213" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="E213" s="2">
         <v>2</v>
@@ -9062,10 +9097,10 @@
         <v>30</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>6</v>
@@ -9100,13 +9135,13 @@
         <v>30</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E215" s="2">
         <v>1</v>
@@ -9138,10 +9173,10 @@
         <v>30</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>20</v>
@@ -9176,10 +9211,10 @@
         <v>30</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>20</v>
@@ -9214,13 +9249,13 @@
         <v>31</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C218" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D218" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="E218" s="2">
         <v>2</v>
@@ -9252,10 +9287,10 @@
         <v>31</v>
       </c>
       <c r="B219" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C219" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>6</v>
@@ -9290,13 +9325,13 @@
         <v>31</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E220" s="2">
         <v>1</v>
@@ -9328,10 +9363,10 @@
         <v>31</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>20</v>
@@ -9366,10 +9401,10 @@
         <v>31</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>20</v>
@@ -9404,10 +9439,10 @@
         <v>31</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>20</v>
@@ -9442,10 +9477,10 @@
         <v>32</v>
       </c>
       <c r="B224" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C224" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>20</v>
@@ -9480,10 +9515,10 @@
         <v>32</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>6</v>
@@ -9518,10 +9553,10 @@
         <v>33</v>
       </c>
       <c r="B226" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C226" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>18</v>
@@ -9556,10 +9591,10 @@
         <v>33</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>20</v>
@@ -9594,10 +9629,10 @@
         <v>33</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>25</v>
@@ -9632,10 +9667,10 @@
         <v>33</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>16</v>
@@ -9670,13 +9705,13 @@
         <v>33</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C230" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D230" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D230" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="E230" s="2">
         <v>4</v>
@@ -9708,10 +9743,10 @@
         <v>33</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>20</v>
@@ -9746,10 +9781,10 @@
         <v>33</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>20</v>
@@ -9784,10 +9819,10 @@
         <v>34</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>6</v>
@@ -9822,10 +9857,10 @@
         <v>34</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>20</v>
@@ -9860,10 +9895,10 @@
         <v>34</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>20</v>
@@ -9898,10 +9933,10 @@
         <v>34</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>20</v>
@@ -9936,7 +9971,7 @@
         <v>34</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>19</v>
@@ -9974,13 +10009,13 @@
         <v>34</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C238" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D238" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D238" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E238" s="2">
         <v>0.5</v>
@@ -10012,7 +10047,7 @@
         <v>34</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>12</v>
@@ -10050,10 +10085,10 @@
         <v>34</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>25</v>
@@ -10088,10 +10123,10 @@
         <v>34</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>25</v>
@@ -10126,10 +10161,10 @@
         <v>34</v>
       </c>
       <c r="B242" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C242" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>16</v>
@@ -10164,10 +10199,10 @@
         <v>35</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>20</v>
@@ -10202,10 +10237,10 @@
         <v>35</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>20</v>
@@ -10240,10 +10275,10 @@
         <v>35</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>20</v>
@@ -10278,10 +10313,10 @@
         <v>35</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>25</v>
@@ -10316,10 +10351,10 @@
         <v>36</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>20</v>
@@ -10354,13 +10389,13 @@
         <v>36</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C248" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D248" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D248" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E248" s="2">
         <v>1</v>
@@ -10392,10 +10427,10 @@
         <v>36</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>20</v>
@@ -10430,7 +10465,7 @@
         <v>36</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>23</v>
@@ -10468,7 +10503,7 @@
         <v>36</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>14</v>
@@ -10506,7 +10541,7 @@
         <v>36</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>15</v>
@@ -10544,10 +10579,10 @@
         <v>37</v>
       </c>
       <c r="B253" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C253" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>6</v>
@@ -10582,10 +10617,10 @@
         <v>37</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>20</v>
@@ -10620,10 +10655,10 @@
         <v>37</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>20</v>
@@ -10658,10 +10693,10 @@
         <v>37</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D256" s="2" t="s">
         <v>25</v>
@@ -10696,10 +10731,10 @@
         <v>37</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>25</v>
@@ -10734,7 +10769,7 @@
         <v>37</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>14</v>
@@ -10772,7 +10807,7 @@
         <v>37</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>15</v>
@@ -10810,10 +10845,10 @@
         <v>38</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>20</v>
@@ -10848,10 +10883,10 @@
         <v>38</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>20</v>
@@ -10886,10 +10921,10 @@
         <v>38</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>20</v>
@@ -10924,10 +10959,10 @@
         <v>38</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>20</v>
@@ -10962,10 +10997,10 @@
         <v>38</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>11</v>
@@ -11000,10 +11035,10 @@
         <v>38</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>20</v>
@@ -11038,7 +11073,7 @@
         <v>38</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>15</v>
@@ -11076,10 +11111,10 @@
         <v>38</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D267" s="2" t="s">
         <v>16</v>
@@ -11114,7 +11149,7 @@
         <v>39</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>9</v>
@@ -11152,10 +11187,10 @@
         <v>39</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>18</v>
@@ -11190,10 +11225,10 @@
         <v>39</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>18</v>
@@ -11228,7 +11263,7 @@
         <v>39</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>19</v>
@@ -11266,7 +11301,7 @@
         <v>39</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>12</v>
@@ -11304,7 +11339,7 @@
         <v>39</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C273" s="2" t="s">
         <v>14</v>
@@ -11342,7 +11377,7 @@
         <v>39</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>15</v>
@@ -11380,10 +11415,10 @@
         <v>39</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>16</v>
@@ -11418,10 +11453,10 @@
         <v>39</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>16</v>
@@ -11456,10 +11491,10 @@
         <v>40</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C277" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="C277" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>20</v>
@@ -11494,13 +11529,13 @@
         <v>40</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E278" s="2">
         <v>2</v>
@@ -11532,10 +11567,10 @@
         <v>40</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>20</v>
@@ -11570,10 +11605,10 @@
         <v>40</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>20</v>
@@ -11608,10 +11643,10 @@
         <v>40</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>25</v>
@@ -11646,10 +11681,10 @@
         <v>40</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>11</v>
@@ -11684,7 +11719,7 @@
         <v>40</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>15</v>
@@ -11722,10 +11757,10 @@
         <v>41</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>6</v>
@@ -11760,10 +11795,10 @@
         <v>41</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>20</v>
@@ -11798,10 +11833,10 @@
         <v>41</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>20</v>
@@ -11836,7 +11871,7 @@
         <v>41</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>19</v>
@@ -11874,10 +11909,10 @@
         <v>41</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>20</v>
@@ -11912,7 +11947,7 @@
         <v>41</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C289" s="2" t="s">
         <v>23</v>
@@ -11950,7 +11985,7 @@
         <v>41</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>14</v>
@@ -11988,7 +12023,7 @@
         <v>41</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>15</v>
@@ -12026,10 +12061,10 @@
         <v>41</v>
       </c>
       <c r="B292" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C292" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>16</v>
@@ -12064,10 +12099,10 @@
         <v>42</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>20</v>
@@ -12102,10 +12137,10 @@
         <v>42</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>20</v>
@@ -12140,10 +12175,10 @@
         <v>42</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>20</v>
@@ -12178,7 +12213,7 @@
         <v>42</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>12</v>
@@ -12216,10 +12251,10 @@
         <v>42</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>11</v>
@@ -12254,10 +12289,10 @@
         <v>42</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>16</v>
@@ -12292,10 +12327,10 @@
         <v>42</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>16</v>
@@ -12330,7 +12365,7 @@
         <v>42</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>14</v>
@@ -12368,7 +12403,7 @@
         <v>42</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>15</v>
@@ -12406,13 +12441,13 @@
         <v>43</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C302" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D302" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D302" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="E302" s="2">
         <v>4</v>
@@ -12444,13 +12479,13 @@
         <v>43</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E303" s="2">
         <v>2</v>
@@ -12482,10 +12517,10 @@
         <v>43</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>20</v>
@@ -12520,10 +12555,10 @@
         <v>43</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D305" s="2" t="s">
         <v>20</v>
@@ -12558,10 +12593,10 @@
         <v>43</v>
       </c>
       <c r="B306" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C306" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C306" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="D306" s="2" t="s">
         <v>18</v>
@@ -12596,7 +12631,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>19</v>
@@ -12634,7 +12669,7 @@
         <v>43</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>23</v>
@@ -12672,10 +12707,10 @@
         <v>43</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>11</v>
@@ -12710,10 +12745,10 @@
         <v>43</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>16</v>
@@ -12748,10 +12783,10 @@
         <v>43</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>20</v>
@@ -12786,10 +12821,10 @@
         <v>43</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D312" s="2" t="s">
         <v>20</v>
@@ -12824,10 +12859,10 @@
         <v>43</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>20</v>
@@ -12862,7 +12897,7 @@
         <v>43</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>14</v>
@@ -12900,7 +12935,7 @@
         <v>43</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>15</v>
@@ -12938,10 +12973,10 @@
         <v>43</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>11</v>
@@ -12976,10 +13011,10 @@
         <v>44</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D317" s="2" t="s">
         <v>20</v>
@@ -13014,10 +13049,10 @@
         <v>44</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>20</v>
@@ -13052,10 +13087,10 @@
         <v>44</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D319" s="2" t="s">
         <v>20</v>
@@ -13090,7 +13125,7 @@
         <v>44</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>19</v>
@@ -13128,10 +13163,10 @@
         <v>44</v>
       </c>
       <c r="B321" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C321" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C321" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="D321" s="2" t="s">
         <v>11</v>
@@ -13166,10 +13201,10 @@
         <v>44</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D322" s="2" t="s">
         <v>20</v>
@@ -13204,7 +13239,7 @@
         <v>44</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>14</v>
@@ -13242,7 +13277,7 @@
         <v>44</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>15</v>
@@ -13280,7 +13315,7 @@
         <v>44</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>23</v>
@@ -13318,10 +13353,10 @@
         <v>44</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D326" s="2" t="s">
         <v>11</v>
@@ -13356,10 +13391,10 @@
         <v>45</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>20</v>
@@ -13394,10 +13429,10 @@
         <v>45</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D328" s="2" t="s">
         <v>20</v>
@@ -13432,10 +13467,10 @@
         <v>45</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D329" s="2" t="s">
         <v>20</v>
@@ -13470,10 +13505,10 @@
         <v>45</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D330" s="2" t="s">
         <v>20</v>
@@ -13508,7 +13543,7 @@
         <v>45</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C331" s="2" t="s">
         <v>19</v>
@@ -13546,10 +13581,10 @@
         <v>45</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D332" s="2" t="s">
         <v>20</v>
@@ -13584,7 +13619,7 @@
         <v>45</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C333" s="2" t="s">
         <v>14</v>
@@ -13622,7 +13657,7 @@
         <v>45</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>15</v>
@@ -13660,10 +13695,10 @@
         <v>45</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D335" s="2" t="s">
         <v>20</v>
@@ -13698,10 +13733,10 @@
         <v>45</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C336" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D336" s="2" t="s">
         <v>20</v>
@@ -13736,10 +13771,10 @@
         <v>45</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C337" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D337" s="2" t="s">
         <v>11</v>
@@ -13770,12 +13805,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L337" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13787,7 +13823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
created separate class to store data in the app
</commit_message>
<xml_diff>
--- a/recipe_db.xlsx
+++ b/recipe_db.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBB30E3-EF98-49D0-A88A-6D27197666D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CFD9A4-EE06-417A-970B-6628D5338BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30960" yWindow="2160" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -978,8 +978,8 @@
   <dimension ref="A1:L337"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>